<commit_message>
closed for certain time
</commit_message>
<xml_diff>
--- a/excel_analysis/nepse outline.xlsx
+++ b/excel_analysis/nepse outline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\OneDrive - ahqb\Pukar Sharma\My Desktop\Stock Market Analysis\NEPSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\gitdemo\AdvancedNEPSE\excel_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EBE663-47D7-48D9-9D77-6924477F6A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5873111D-F692-4A86-A455-70C7BA2F2667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5760" yWindow="228" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" r:id="rId1"/>
@@ -465,37 +465,11 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -557,6 +531,39 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -567,13 +574,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3118,20 +3118,20 @@
   <autoFilter ref="C3:Q25" xr:uid="{06AF2333-7BFD-4614-ADA2-9B81E331D208}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{E1A292DA-0E6E-42D8-ADD8-188800BC3205}" name="Month-" totalsRowLabel="Monthly average"/>
-    <tableColumn id="2" xr3:uid="{3AE553CD-B203-461B-9F91-EA40F8088CF7}" name="Jan" totalsRowFunction="average" dataDxfId="27" totalsRowDxfId="13" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{2996653D-9DA2-47FE-95DA-A1B8649CD20D}" name="Feb" totalsRowFunction="average" dataDxfId="26" totalsRowDxfId="12" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{5699D38D-F259-4726-AAAA-031C4ABDF5B6}" name="Mar" totalsRowFunction="average" dataDxfId="25" totalsRowDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{F6E39866-E897-4325-9C12-7C1032F77ADE}" name="Apr" totalsRowFunction="average" dataDxfId="24" totalsRowDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{C787AE25-3003-4BC7-9724-F298716B0178}" name="May" totalsRowFunction="average" dataDxfId="23" totalsRowDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{7962F693-C966-4A35-AA17-38B8E317A33F}" name="Jun" totalsRowFunction="average" dataDxfId="22" totalsRowDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{A3F268D2-DB26-4EDA-A25E-757C235B38A8}" name="Jul" totalsRowFunction="average" dataDxfId="21" totalsRowDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{70255B97-EAD7-4F73-8E29-9A4A25D39D33}" name="Aug" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="10" xr3:uid="{CF289C80-0DA1-4C92-ABF6-CB4D9D19D016}" name="Sep" totalsRowFunction="average" dataDxfId="19" totalsRowDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="11" xr3:uid="{3E8997FC-C6D7-4940-B0C7-9BDE5055C260}" name="Oct" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{FCA4AF4E-E6D8-429E-95CD-EBC8F2BF924D}" name="Nov" totalsRowFunction="average" dataDxfId="17" totalsRowDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="13" xr3:uid="{28EF217B-AF3D-47AB-97CA-CC032CCE28B4}" name="Dec" totalsRowFunction="average" dataDxfId="16" totalsRowDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="14" xr3:uid="{CE7C4BAF-E226-4170-B4DC-B3E603C3BA0C}" name="Yearly Average" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="15" xr3:uid="{CFFFF854-8E54-4173-91AC-C22B3A417A22}" name="Yearly sum" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{3AE553CD-B203-461B-9F91-EA40F8088CF7}" name="Jan" totalsRowFunction="average" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{2996653D-9DA2-47FE-95DA-A1B8649CD20D}" name="Feb" totalsRowFunction="average" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{5699D38D-F259-4726-AAAA-031C4ABDF5B6}" name="Mar" totalsRowFunction="average" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{F6E39866-E897-4325-9C12-7C1032F77ADE}" name="Apr" totalsRowFunction="average" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{C787AE25-3003-4BC7-9724-F298716B0178}" name="May" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{7962F693-C966-4A35-AA17-38B8E317A33F}" name="Jun" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{A3F268D2-DB26-4EDA-A25E-757C235B38A8}" name="Jul" totalsRowFunction="average" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{70255B97-EAD7-4F73-8E29-9A4A25D39D33}" name="Aug" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="10" xr3:uid="{CF289C80-0DA1-4C92-ABF6-CB4D9D19D016}" name="Sep" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{3E8997FC-C6D7-4940-B0C7-9BDE5055C260}" name="Oct" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{FCA4AF4E-E6D8-429E-95CD-EBC8F2BF924D}" name="Nov" totalsRowFunction="average" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="13" xr3:uid="{28EF217B-AF3D-47AB-97CA-CC032CCE28B4}" name="Dec" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="14" xr3:uid="{CE7C4BAF-E226-4170-B4DC-B3E603C3BA0C}" name="Yearly Average" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="15" xr3:uid="{CFFFF854-8E54-4173-91AC-C22B3A417A22}" name="Yearly sum" totalsRowFunction="average" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3416,7 +3416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3672,8 +3672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1DC02A4-5B4C-4DD9-A3B2-7DC4058A8632}">
   <dimension ref="C3:W268"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5478,7 +5478,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="D5:O25">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">

</xml_diff>